<commit_message>
Create and Edit Profile implemented
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="95">
   <si>
     <t>Email</t>
   </si>
@@ -695,7 +695,7 @@
       <c r="B4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>